<commit_message>
Figure and Table updates
</commit_message>
<xml_diff>
--- a/doc/tables/Table1.xlsx
+++ b/doc/tables/Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamklie/Desktop/lab/projects/predictMEE/doc/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5AECB81B-CF72-3A49-9D94-205C0B307ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CB9F194C-75AA-B64F-ABA2-2E75AAE87955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440"/>
+    <workbookView xWindow="-29280" yWindow="4600" windowWidth="28040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="3" r:id="rId1"/>
@@ -404,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -520,6 +520,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -535,7 +544,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -550,108 +559,53 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -701,16 +655,16 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -756,7 +710,28 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -821,9 +796,7 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -846,21 +819,15 @@
         <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="thin">
+        <right style="medium">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top style="medium">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -892,17 +859,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A1:E11"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
-    <sortCondition descending="1" ref="E1:E11"/>
+    <sortCondition ref="A1:A11"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="Class Name" dataDxfId="4"/>
     <tableColumn id="2" name="# TITLES" dataDxfId="3"/>
     <tableColumn id="3" name="# Predicted" dataDxfId="2"/>
-    <tableColumn id="5" name="# Correct" dataDxfId="0"/>
-    <tableColumn id="4" name="Accuracy" dataDxfId="1"/>
+    <tableColumn id="5" name="# Correct" dataDxfId="1"/>
+    <tableColumn id="4" name="Accuracy" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1208,7 +1175,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E11" sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1218,13 +1185,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1235,177 +1202,178 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4">
-        <v>190</v>
-      </c>
-      <c r="C2" s="4">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="5">
+        <v>224</v>
+      </c>
+      <c r="D2" s="2">
+        <v>106</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.47321428571428498</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C3" s="2">
-        <v>855</v>
-      </c>
-      <c r="D3" s="7">
-        <v>787</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.92046783625730999</v>
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>702</v>
+      </c>
+      <c r="C3" s="4">
+        <v>144</v>
+      </c>
+      <c r="D3" s="2">
+        <v>68</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.47222222222222199</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>122</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>23</v>
       </c>
-      <c r="D4" s="7">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.86956521739130399</v>
+      <c r="D4" s="2">
+        <v>22</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.95652173913043403</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="2">
-        <v>295</v>
-      </c>
-      <c r="D5" s="7">
-        <v>241</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.81694915254237199</v>
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>78</v>
+      </c>
+      <c r="C5" s="4">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.83333333333333304</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>702</v>
-      </c>
-      <c r="C6" s="2">
-        <v>144</v>
-      </c>
-      <c r="D6" s="7">
-        <v>56</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.38888888888888801</v>
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>595</v>
+      </c>
+      <c r="C6" s="4">
+        <v>130</v>
+      </c>
+      <c r="D6" s="2">
+        <v>81</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.62307692307692297</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2">
-        <v>595</v>
-      </c>
-      <c r="C7" s="2">
-        <v>130</v>
-      </c>
-      <c r="D7" s="7">
-        <v>49</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.37692307692307597</v>
+      <c r="A7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>275</v>
+      </c>
+      <c r="C7" s="4">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.36666666666666597</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C8" s="2">
-        <v>237</v>
-      </c>
-      <c r="D8" s="7">
-        <v>88</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.37130801687763698</v>
+      <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>190</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
         <v>1000</v>
       </c>
-      <c r="C9" s="2">
-        <v>224</v>
-      </c>
-      <c r="D9" s="7">
-        <v>71</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.31696428571428498</v>
+      <c r="C9" s="4">
+        <v>855</v>
+      </c>
+      <c r="D9" s="2">
+        <v>811</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.94853801169590601</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2">
-        <v>275</v>
-      </c>
-      <c r="C10" s="2">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="4">
+        <v>295</v>
+      </c>
+      <c r="D10" s="2">
+        <v>242</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.82033898305084696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" thickBot="1">
-      <c r="A11" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="B11" s="9">
-        <v>78</v>
+        <v>1000</v>
       </c>
       <c r="C11" s="9">
-        <v>12</v>
-      </c>
-      <c r="D11" s="10">
-        <v>2</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.16666666666666599</v>
+        <v>237</v>
+      </c>
+      <c r="D11" s="2">
+        <v>151</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.63713080168776304</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>